<commit_message>
add comments when first column starts with #.
- 1_excel.pl : # this is comments.  (1_excel.pl ignores this row as comments when starts with #.)
- 1_example.xlsx : example
</commit_message>
<xml_diff>
--- a/1_example.xlsx
+++ b/1_example.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\code\github\CGA_RDL\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="25596" windowHeight="14976" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>DID_WORK_FOR_DEFINE_0</t>
   </si>
@@ -148,17 +153,21 @@
   </si>
   <si>
     <t>VALUE</t>
+  </si>
+  <si>
+    <t># this is comments.  (1_excel.pl ignores this row as comments when starts with #.)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -182,7 +191,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -190,8 +199,15 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -234,22 +250,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="하이퍼링크" xfId="11" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -286,7 +310,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -632,24 +656,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
@@ -657,7 +681,7 @@
       <c r="F1" s="2"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
@@ -665,7 +689,7 @@
       <c r="F2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -673,31 +697,31 @@
       <c r="F3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="C4" s="1"/>
       <c r="F4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="C5" s="1"/>
       <c r="F5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="C6" s="1"/>
       <c r="F6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="C7" s="1"/>
       <c r="F7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -707,7 +731,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -717,7 +741,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -728,7 +752,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -739,7 +763,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -751,7 +775,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -762,10 +786,15 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="3"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -773,7 +802,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -781,7 +810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -789,7 +818,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -797,19 +826,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>38</v>
       </c>
@@ -817,7 +846,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
@@ -825,7 +854,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
@@ -833,37 +862,37 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -871,7 +900,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>20</v>
       </c>
@@ -879,7 +908,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>23</v>
       </c>
@@ -887,7 +916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>17</v>
       </c>
@@ -895,7 +924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>14</v>
       </c>
@@ -903,7 +932,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>9</v>
       </c>
@@ -911,69 +940,70 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Support a single variable. $VARIABLE{?}
- Issue : I wanna get single variable not hash. #12
	- modified:   1_example.xlsx
        - example  [VARIABLE]Name
	- modified:   1_excel.pl
        - process [VARIABLE]tag
</commit_message>
<xml_diff>
--- a/1_example.xlsx
+++ b/1_example.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="25596" windowHeight="14976" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="25596" windowHeight="14976" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>DID_WORK_FOR_DEFINE_0</t>
   </si>
@@ -156,6 +156,18 @@
   </si>
   <si>
     <t># this is comments.  (1_excel.pl ignores this row as comments when starts with #.)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>[VARIABLE]Name</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>1434bam</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>#this is a single variable not hash.  +&lt;+$VARIABLE{"Name"}+&gt;+</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -163,7 +175,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -210,6 +222,12 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -243,11 +261,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="열어 본 하이퍼링크" xfId="2" builtinId="9" hidden="1"/>
@@ -657,7 +676,7 @@
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
@@ -710,19 +729,26 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="F6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="F7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="1"/>
+      <c r="A8" s="4"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>

</xml_diff>

<commit_message>
add file : excel_version & update excel file
</commit_message>
<xml_diff>
--- a/1_example.xlsx
+++ b/1_example.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\code\github\CGA_RDL\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="25596" windowHeight="14976" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
   <si>
     <t>DID_WORK_FOR_DEFINE_0</t>
   </si>
@@ -169,18 +164,52 @@
   <si>
     <t>#this is a single variable not hash.  +&lt;+$VARIABLE{"Name"}+&gt;+</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>[VARIABLE]Excel_Version</t>
+  </si>
+  <si>
+    <t>v2.0.1</t>
+  </si>
+  <si>
+    <t>[VARIABLE]CDA_RDL_Version</t>
+  </si>
+  <si>
+    <t>v1.0.2</t>
+  </si>
+  <si>
+    <t>#this is a single variable not hash.  +&lt;+$VARIABLE{"Date"}+&gt;+</t>
+  </si>
+  <si>
+    <t>#this is update time of  header each file.</t>
+  </si>
+  <si>
+    <t>[VARIABLE]Version</t>
+  </si>
+  <si>
+    <t>2.0.00</t>
+  </si>
+  <si>
+    <t>[VARIABLE]Date</t>
+  </si>
+  <si>
+    <t>2020.02.13</t>
+  </si>
+  <si>
+    <t># it is related to the verion of excel_version file.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -203,7 +232,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -211,13 +240,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -228,16 +257,53 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -245,8 +311,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -260,28 +354,40 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
-    <cellStyle name="열어 본 하이퍼링크" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="11" builtinId="8" hidden="1"/>
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -302,13 +408,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -329,7 +435,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -673,363 +779,411 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" ht="16" thickBot="1">
+      <c r="A2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" ht="17" thickTop="1" thickBot="1">
+      <c r="A3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="17" thickTop="1" thickBot="1">
+      <c r="A4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="17" thickTop="1" thickBot="1">
+      <c r="A5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="17" thickTop="1" thickBot="1">
+      <c r="A6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16" thickTop="1"/>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="F1" s="2"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+      <c r="C8" s="1"/>
+      <c r="F8" s="2"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="4"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" s="1"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="4"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" s="1" t="s">
+    <row r="33" spans="1:2">
+      <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" s="1" t="s">
+    <row r="34" spans="1:2">
+      <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" s="1" t="s">
+    <row r="35" spans="1:2">
+      <c r="A35" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" s="1" t="s">
+    <row r="36" spans="1:2">
+      <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" s="1" t="s">
+    <row r="37" spans="1:2">
+      <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" s="1" t="s">
+    <row r="38" spans="1:2">
+      <c r="A38" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" s="1" t="s">
+    <row r="39" spans="1:2">
+      <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="1" t="s">
+    <row r="40" spans="1:2">
+      <c r="A40" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A38" s="1" t="s">
+    <row r="45" spans="1:2">
+      <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B45" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A39" s="1" t="s">
+    <row r="46" spans="1:2">
+      <c r="A46" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A40" s="1" t="s">
+    <row r="47" spans="1:2">
+      <c r="A47" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A41" s="1" t="s">
+    <row r="48" spans="1:2">
+      <c r="A48" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A42" s="1" t="s">
+    <row r="49" spans="1:2">
+      <c r="A49" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43" s="1" t="s">
+    <row r="50" spans="1:2">
+      <c r="A50" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A48" s="1" t="s">
+    <row r="51" spans="1:2">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A49" s="1" t="s">
+    <row r="56" spans="1:2">
+      <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A50" s="1" t="s">
+    <row r="57" spans="1:2">
+      <c r="A57" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A51" s="1" t="s">
+    <row r="58" spans="1:2">
+      <c r="A58" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A52" s="1" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A53" s="1" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A54" s="1" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A55" s="1" t="s">
+    <row r="62" spans="1:2">
+      <c r="A62" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A56" s="1" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A57" s="1" t="s">
+    <row r="64" spans="1:2">
+      <c r="A64" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A58" s="1" t="s">
+    <row r="65" spans="1:1">
+      <c r="A65" s="1" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>